<commit_message>
Done(for now) with the assembler working on some new docs for the programing lang done(for now) with the filesystem working on the core Emulator updated the spces (now in INSTRUCTIONS.txt)
</commit_message>
<xml_diff>
--- a/BES-8-CPU/CPU-SPECS/Stack.xlsx
+++ b/BES-8-CPU/CPU-SPECS/Stack.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjorn\Desktop\CPUs\BES-8-CPU\CPU-SPECS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74065774-E226-4B64-8F56-747F2A44B16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5060E99B-BCBD-4E64-B7B9-B7A6B7777938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{60BD8EC7-1CE0-4AB1-8C1D-843B2C9E47D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{60BD8EC7-1CE0-4AB1-8C1D-843B2C9E47D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Int 10h calls" sheetId="3" r:id="rId3"/>
-    <sheet name="Int 13h calls" sheetId="4" r:id="rId4"/>
+    <sheet name="Interrupt Instr" sheetId="5" r:id="rId3"/>
+    <sheet name="Int 10h calls" sheetId="3" r:id="rId4"/>
+    <sheet name="Int 13h calls" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
   <si>
     <t>A</t>
   </si>
@@ -209,9 +210,6 @@
     <t>Hedder Disk</t>
   </si>
   <si>
-    <t>Disk 1</t>
-  </si>
-  <si>
     <t>Data Out</t>
   </si>
   <si>
@@ -351,6 +349,78 @@
   </si>
   <si>
     <t>byte Bank</t>
+  </si>
+  <si>
+    <t>Disk 0</t>
+  </si>
+  <si>
+    <t>Interrupt</t>
+  </si>
+  <si>
+    <t>short Exit code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Console Text Output </t>
+  </si>
+  <si>
+    <t>Char c</t>
+  </si>
+  <si>
+    <t>short CX</t>
+  </si>
+  <si>
+    <t>short CY</t>
+  </si>
+  <si>
+    <t>byte color</t>
+  </si>
+  <si>
+    <t>ushort data</t>
+  </si>
+  <si>
+    <t>ushort addr</t>
+  </si>
+  <si>
+    <t>return char</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>byte disk</t>
+  </si>
+  <si>
+    <t>Read Sector</t>
+  </si>
+  <si>
+    <t>byte sector</t>
+  </si>
+  <si>
+    <t>Conv hex to dec</t>
+  </si>
+  <si>
+    <t>char* hexstr</t>
+  </si>
+  <si>
+    <t>return ushort dec</t>
+  </si>
+  <si>
+    <t>Write Count</t>
+  </si>
+  <si>
+    <t>ushort* data</t>
+  </si>
+  <si>
+    <t>ushort count</t>
+  </si>
+  <si>
+    <t>ushort StartAddr</t>
+  </si>
+  <si>
+    <t>short addr</t>
+  </si>
+  <si>
+    <t>short page</t>
   </si>
 </sst>
 </file>
@@ -374,7 +444,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -382,11 +452,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,9 +502,26 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BEBC3B-EE35-4293-8A08-F90136BE72E0}">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,8 +910,8 @@
         <f>DEC2HEX(N2)</f>
         <v>FF85</v>
       </c>
-      <c r="P2" t="s">
-        <v>31</v>
+      <c r="Q2" t="s">
+        <v>7</v>
       </c>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
@@ -805,9 +929,6 @@
         <f t="shared" ref="O3:O30" si="0">DEC2HEX(N3)</f>
         <v>FF84</v>
       </c>
-      <c r="P3" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N4" s="1">
@@ -817,13 +938,10 @@
         <f t="shared" si="0"/>
         <v>FF83</v>
       </c>
-      <c r="P4" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N5" s="1">
         <v>65410</v>
@@ -832,9 +950,6 @@
         <f t="shared" si="0"/>
         <v>FF82</v>
       </c>
-      <c r="P5" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -847,7 +962,7 @@
         <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N6" s="1">
         <v>65409</v>
@@ -856,9 +971,6 @@
         <f t="shared" si="0"/>
         <v>FF81</v>
       </c>
-      <c r="P6" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -866,7 +978,7 @@
       </c>
       <c r="B7" t="str">
         <f>DEC2HEX(HEX2DEC(_xlfn.CONCAT($C$8,$C$9)),4)</f>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="I7" t="str">
         <f>DEC2HEX(J7)</f>
@@ -882,12 +994,6 @@
         <f t="shared" si="0"/>
         <v>FF80</v>
       </c>
-      <c r="P7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -916,7 +1022,7 @@
         <v>40</v>
       </c>
       <c r="C9">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
@@ -1275,7 +1381,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I24">
         <v>41010</v>
@@ -1306,7 +1412,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I25">
         <v>41011</v>
@@ -1336,7 +1442,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I26">
         <v>41012</v>
@@ -1371,11 +1477,18 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="str">
+        <f>DEC2HEX(HEX2DEC(_xlfn.CONCAT(C29,C30)),4)</f>
+        <v>0000</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="J28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N28" s="1">
         <v>65387</v>
@@ -1386,14 +1499,11 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" t="s">
-        <v>58</v>
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -1421,15 +1531,9 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30">
+        <v>51</v>
+      </c>
+      <c r="C30">
         <v>0</v>
       </c>
       <c r="F30" s="1"/>
@@ -1442,10 +1546,10 @@
         <v>225281</v>
       </c>
       <c r="K30" t="s">
+        <v>89</v>
+      </c>
+      <c r="L30" t="s">
         <v>90</v>
-      </c>
-      <c r="L30" t="s">
-        <v>91</v>
       </c>
       <c r="N30" s="1">
         <v>65385</v>
@@ -1456,18 +1560,6 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1481,7 +1573,7 @@
         <v>53</v>
       </c>
       <c r="L31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -1498,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1513,6 +1605,15 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1524,6 +1625,18 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -1536,10 +1649,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1551,28 +1664,42 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37">
-        <v>11</v>
-      </c>
-      <c r="C37">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41">
+        <v>16</v>
+      </c>
+      <c r="C41">
         <v>0</v>
       </c>
-      <c r="D37">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42">
+        <v>17</v>
+      </c>
+      <c r="C42">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>12</v>
-      </c>
-      <c r="C38">
+      <c r="D42">
         <v>0</v>
       </c>
-      <c r="D38">
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>18</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
         <v>0</v>
       </c>
     </row>
@@ -1585,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4B0602-ED20-46AA-BDD0-0BE83C63CF25}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1969,77 +2096,108 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0253E003-5A06-488A-A834-EFA5548C0B3D}">
-  <dimension ref="A1:V46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB048CF3-8843-4B40-B9E5-99F22F345F1B}">
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" style="1" customWidth="1"/>
-    <col min="2" max="9" width="9.140625" style="1"/>
+    <col min="1" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" customWidth="1"/>
+    <col min="29" max="29" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="R1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="S1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="str">
+        <f>DEC2HEX(A2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="7"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -2050,56 +2208,70 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="str">
+        <f t="shared" ref="C3:C16" si="0">DEC2HEX(A3)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N3" s="7"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="4"/>
+      <c r="S3" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="V3" s="7"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -2112,11 +2284,27 @@
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -2129,11 +2317,27 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -2146,11 +2350,27 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -2163,28 +2383,66 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="L8" s="7"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
+      <c r="S8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="T8" s="7"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -2197,11 +2455,27 @@
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -2214,11 +2488,27 @@
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -2231,83 +2521,199 @@
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" s="7"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="Q12" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="R12" s="11"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="W12" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="R13" s="11"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="P15" s="7"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
+      <c r="S15" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="T15" s="7"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -2316,15 +2722,31 @@
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="str">
+        <f t="shared" ref="C17:C28" si="1">DEC2HEX(A17)</f>
+        <v>F</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -2333,15 +2755,31 @@
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
@@ -2350,15 +2788,31 @@
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
@@ -2367,15 +2821,31 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>18</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
@@ -2384,24 +2854,31 @@
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="4">
-        <v>20</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
@@ -2410,15 +2887,31 @@
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -2427,15 +2920,31 @@
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -2444,15 +2953,31 @@
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
@@ -2461,15 +2986,31 @@
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
@@ -2478,15 +3019,31 @@
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
@@ -2495,15 +3052,31 @@
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
@@ -2512,15 +3085,31 @@
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>26</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>1A</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
@@ -2529,297 +3118,1205 @@
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="100">
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0253E003-5A06-488A-A834-EFA5548C0B3D}">
+  <dimension ref="A1:V46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.42578125" style="1" customWidth="1"/>
+    <col min="2" max="9" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="10">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="10">
+        <v>20</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-      <c r="V38" s="4"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
-      <c r="U41" s="4"/>
-      <c r="V41" s="4"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10"/>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
-      <c r="T42" s="4"/>
-      <c r="U42" s="4"/>
-      <c r="V42" s="4"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
-      <c r="T43" s="4"/>
-      <c r="U43" s="4"/>
-      <c r="V43" s="4"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
-      <c r="V44" s="4"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="10"/>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
-      <c r="V45" s="4"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="10"/>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
-      <c r="T46" s="4"/>
-      <c r="U46" s="4"/>
-      <c r="V46" s="4"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="10"/>
+      <c r="V46" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="J15:V15"/>
+    <mergeCell ref="J16:V16"/>
+    <mergeCell ref="J17:V17"/>
+    <mergeCell ref="J18:V18"/>
+    <mergeCell ref="J19:V19"/>
+    <mergeCell ref="J20:V20"/>
+    <mergeCell ref="J21:V21"/>
+    <mergeCell ref="J22:V22"/>
+    <mergeCell ref="J23:V23"/>
+    <mergeCell ref="J24:V24"/>
+    <mergeCell ref="J25:V25"/>
+    <mergeCell ref="J26:V26"/>
+    <mergeCell ref="J27:V27"/>
+    <mergeCell ref="J28:V28"/>
+    <mergeCell ref="J29:V29"/>
+    <mergeCell ref="J33:V33"/>
+    <mergeCell ref="J34:V34"/>
+    <mergeCell ref="J1:V1"/>
+    <mergeCell ref="J2:V2"/>
+    <mergeCell ref="J3:V3"/>
+    <mergeCell ref="J4:V4"/>
+    <mergeCell ref="J5:V5"/>
+    <mergeCell ref="J6:V6"/>
+    <mergeCell ref="J7:V7"/>
+    <mergeCell ref="J8:V8"/>
+    <mergeCell ref="J9:V9"/>
+    <mergeCell ref="J10:V10"/>
+    <mergeCell ref="J11:V11"/>
+    <mergeCell ref="J12:V12"/>
+    <mergeCell ref="J13:V13"/>
+    <mergeCell ref="J14:V14"/>
     <mergeCell ref="J45:V45"/>
     <mergeCell ref="J46:V46"/>
     <mergeCell ref="D21:E21"/>
@@ -2836,79 +4333,12 @@
     <mergeCell ref="J30:V30"/>
     <mergeCell ref="J31:V31"/>
     <mergeCell ref="J32:V32"/>
-    <mergeCell ref="J33:V33"/>
-    <mergeCell ref="J34:V34"/>
-    <mergeCell ref="J1:V1"/>
-    <mergeCell ref="J2:V2"/>
-    <mergeCell ref="J3:V3"/>
-    <mergeCell ref="J4:V4"/>
-    <mergeCell ref="J5:V5"/>
-    <mergeCell ref="J6:V6"/>
-    <mergeCell ref="J7:V7"/>
-    <mergeCell ref="J8:V8"/>
-    <mergeCell ref="J9:V9"/>
-    <mergeCell ref="J10:V10"/>
-    <mergeCell ref="J11:V11"/>
-    <mergeCell ref="J12:V12"/>
-    <mergeCell ref="J13:V13"/>
-    <mergeCell ref="J14:V14"/>
-    <mergeCell ref="J25:V25"/>
-    <mergeCell ref="J26:V26"/>
-    <mergeCell ref="J27:V27"/>
-    <mergeCell ref="J28:V28"/>
-    <mergeCell ref="J29:V29"/>
-    <mergeCell ref="J20:V20"/>
-    <mergeCell ref="J21:V21"/>
-    <mergeCell ref="J22:V22"/>
-    <mergeCell ref="J23:V23"/>
-    <mergeCell ref="J24:V24"/>
-    <mergeCell ref="J15:V15"/>
-    <mergeCell ref="J16:V16"/>
-    <mergeCell ref="J17:V17"/>
-    <mergeCell ref="J18:V18"/>
-    <mergeCell ref="J19:V19"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F820F2B8-A0D6-407B-8331-DFA89AFEF3E6}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
@@ -2925,7 +4355,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>40</v>
@@ -2951,250 +4381,251 @@
       <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="J1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="G2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="G2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="4">
+        <v>71</v>
+      </c>
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="4"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="10"/>
       <c r="G3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="4">
+        <v>72</v>
+      </c>
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="4"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="10"/>
       <c r="F4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="10">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="4">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="10"/>
+      <c r="J5" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="10">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="4">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="4">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="J6:Z6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J5:Z5"/>
+    <mergeCell ref="J3:Z3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="J4:Z4"/>
+    <mergeCell ref="J1:Z1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="J2:Z2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -3204,14 +4635,13 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="J5:Z5"/>
-    <mergeCell ref="J3:Z3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="J4:Z4"/>
-    <mergeCell ref="J1:Z1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="J2:Z2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="J6:Z6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Assembly Language is now done rework of the compiler
</commit_message>
<xml_diff>
--- a/BES-8-CPU/CPU-SPECS/Stack.xlsx
+++ b/BES-8-CPU/CPU-SPECS/Stack.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjorn\Desktop\CPUs\BES-8-CPU\CPU-SPECS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5060E99B-BCBD-4E64-B7B9-B7A6B7777938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9DB38C-D188-4C45-970C-D2A8D6820FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{60BD8EC7-1CE0-4AB1-8C1D-843B2C9E47D7}"/>
+    <workbookView xWindow="12495" yWindow="0" windowWidth="12810" windowHeight="15135" activeTab="1" xr2:uid="{60BD8EC7-1CE0-4AB1-8C1D-843B2C9E47D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Interrupt Instr" sheetId="5" r:id="rId3"/>
-    <sheet name="Int 10h calls" sheetId="3" r:id="rId4"/>
-    <sheet name="Int 13h calls" sheetId="4" r:id="rId5"/>
+    <sheet name="TestProgram" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Interrupt Instr" sheetId="5" r:id="rId4"/>
+    <sheet name="Int 10h calls" sheetId="3" r:id="rId5"/>
+    <sheet name="Int 13h calls" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="128">
   <si>
     <t>A</t>
   </si>
@@ -421,6 +422,9 @@
   </si>
   <si>
     <t>short page</t>
+  </si>
+  <si>
+    <t>e8</t>
   </si>
 </sst>
 </file>
@@ -493,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -509,19 +513,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,7 +842,7 @@
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="F31" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,11 +1712,884 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFC2456-8F03-4C66-81C2-5B49407479C5}">
+  <dimension ref="A1:X43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="3.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="7"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" t="str">
+        <f>DEC2HEX(N2)</f>
+        <v>1</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="T2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="7"/>
+      <c r="W2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="7"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="N3" s="1">
+        <v>2</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O30" si="0">DEC2HEX(N3)</f>
+        <v>2</v>
+      </c>
+      <c r="T3" t="str">
+        <f>DEC2HEX(U3)</f>
+        <v>32000</v>
+      </c>
+      <c r="U3">
+        <v>204800</v>
+      </c>
+      <c r="W3">
+        <v>32000</v>
+      </c>
+      <c r="X3">
+        <f>HEX2DEC(W3)</f>
+        <v>204800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N4" s="1">
+        <v>3</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" ref="T4:T18" si="1">DEC2HEX(U4)</f>
+        <v>32001</v>
+      </c>
+      <c r="U4">
+        <v>204801</v>
+      </c>
+      <c r="W4">
+        <v>32001</v>
+      </c>
+      <c r="X4">
+        <v>225281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N5" s="1">
+        <v>4</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="1"/>
+        <v>32002</v>
+      </c>
+      <c r="U5">
+        <v>204802</v>
+      </c>
+      <c r="W5">
+        <v>32002</v>
+      </c>
+      <c r="X5">
+        <v>225282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="1"/>
+        <v>32003</v>
+      </c>
+      <c r="U6">
+        <v>204803</v>
+      </c>
+      <c r="W6">
+        <v>32003</v>
+      </c>
+      <c r="X6">
+        <v>225283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IF(B7&lt;&gt;0,LOOKUP(HEX2DEC(B7),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C8),2),DEC2HEX(HEX2DEC(C9),2)))</f>
+        <v>03E8</v>
+      </c>
+      <c r="N7" s="1">
+        <v>6</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="1"/>
+        <v>32004</v>
+      </c>
+      <c r="U7">
+        <v>204804</v>
+      </c>
+      <c r="W7">
+        <v>32004</v>
+      </c>
+      <c r="X7">
+        <v>225284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="N8" s="1">
+        <v>7</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="1"/>
+        <v>32005</v>
+      </c>
+      <c r="U8">
+        <v>204805</v>
+      </c>
+      <c r="W8">
+        <v>32005</v>
+      </c>
+      <c r="X8">
+        <v>225285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>127</v>
+      </c>
+      <c r="N9" s="1">
+        <v>8</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="1"/>
+        <v>32006</v>
+      </c>
+      <c r="U9">
+        <v>204806</v>
+      </c>
+      <c r="W9">
+        <v>32006</v>
+      </c>
+      <c r="X9">
+        <v>225286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="str">
+        <f>IF(B10&lt;&gt;0,LOOKUP(HEX2DEC(B10),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C11),2),DEC2HEX(HEX2DEC(C12),2)))</f>
+        <v>0000</v>
+      </c>
+      <c r="N10" s="1">
+        <v>9</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="1"/>
+        <v>32007</v>
+      </c>
+      <c r="U10">
+        <v>204807</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>10</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="1"/>
+        <v>32008</v>
+      </c>
+      <c r="U11">
+        <v>204808</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="N12" s="1">
+        <v>11</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="1"/>
+        <v>32009</v>
+      </c>
+      <c r="U12">
+        <v>204809</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="str">
+        <f>IF(B13&lt;&gt;0,LOOKUP(HEX2DEC(B13),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C14),2),DEC2HEX(HEX2DEC(C15),2)))</f>
+        <v>0000</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="N13" s="1">
+        <v>12</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="T13" t="str">
+        <f t="shared" si="1"/>
+        <v>3200A</v>
+      </c>
+      <c r="U13">
+        <v>204810</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="N14" s="1">
+        <v>13</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" si="1"/>
+        <v>3200B</v>
+      </c>
+      <c r="U14">
+        <v>204811</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="N15" s="1">
+        <v>14</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="1"/>
+        <v>3200C</v>
+      </c>
+      <c r="U15">
+        <v>204812</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="str">
+        <f>IF(B16&lt;&gt;0,LOOKUP(HEX2DEC(B16),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C17),2),DEC2HEX(HEX2DEC(C18),2)))</f>
+        <v>0000</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="N16" s="1">
+        <v>15</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="0"/>
+        <v>F</v>
+      </c>
+      <c r="T16" t="str">
+        <f t="shared" si="1"/>
+        <v>3200D</v>
+      </c>
+      <c r="U16">
+        <v>204813</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="N17" s="1">
+        <v>16</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" si="1"/>
+        <v>3200E</v>
+      </c>
+      <c r="U17">
+        <v>204814</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="I18">
+        <v>11000</v>
+      </c>
+      <c r="J18">
+        <v>30</v>
+      </c>
+      <c r="N18" s="1">
+        <v>17</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="1"/>
+        <v>3200F</v>
+      </c>
+      <c r="U18">
+        <v>204815</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="str">
+        <f>IF(B19&lt;&gt;0,LOOKUP(HEX2DEC(B19),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C20),2),DEC2HEX(HEX2DEC(C21),2)))</f>
+        <v>0000</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="I19">
+        <v>11001</v>
+      </c>
+      <c r="J19">
+        <v>20</v>
+      </c>
+      <c r="N19" s="1">
+        <v>18</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="I20">
+        <v>11002</v>
+      </c>
+      <c r="J20">
+        <v>10</v>
+      </c>
+      <c r="N20" s="1">
+        <v>19</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="N21" s="1">
+        <v>20</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="str">
+        <f>IF(B22&lt;&gt;0,LOOKUP(HEX2DEC(B22),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C23),2),DEC2HEX(HEX2DEC(C24),2)))</f>
+        <v>0000</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="N22" s="1">
+        <v>21</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="N23" s="1">
+        <v>22</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" t="s">
+        <v>82</v>
+      </c>
+      <c r="I24">
+        <v>41010</v>
+      </c>
+      <c r="J24">
+        <f>HEX2DEC(I24)</f>
+        <v>266256</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>23</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="str">
+        <f>IF(B25&lt;&gt;0,LOOKUP(HEX2DEC(B25),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C26),2),DEC2HEX(HEX2DEC(C27),2)))</f>
+        <v>0000</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25">
+        <v>41011</v>
+      </c>
+      <c r="J25">
+        <f t="shared" ref="J25:J26" si="2">HEX2DEC(I25)</f>
+        <v>266257</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1">
+        <v>24</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26">
+        <v>41012</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>266258</v>
+      </c>
+      <c r="N26" s="1">
+        <v>25</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="N27" s="1">
+        <v>26</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="0"/>
+        <v>1A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="str">
+        <f>IF(B28&lt;&gt;0,LOOKUP(HEX2DEC(B28),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C29),2),DEC2HEX(HEX2DEC(C30),2)))</f>
+        <v>0000</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="N28" s="1">
+        <v>27</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="0"/>
+        <v>1B</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="N29" s="1">
+        <v>28</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="0"/>
+        <v>1C</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="N30" s="1">
+        <v>29</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="0"/>
+        <v>1D</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41">
+        <v>16</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42">
+        <v>17</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>18</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4B0602-ED20-46AA-BDD0-0BE83C63CF25}">
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D9" sqref="D8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,12 +2971,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB048CF3-8843-4B40-B9E5-99F22F345F1B}">
   <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:P13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,19 +2994,19 @@
       <c r="A1" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
       <c r="K1" s="4" t="s">
         <v>40</v>
       </c>
@@ -2180,24 +3056,24 @@
       <c r="A2" s="9">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7" t="str">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="str">
         <f>DEC2HEX(A2)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -2217,40 +3093,40 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7" t="str">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="str">
         <f t="shared" ref="C3:C16" si="0">DEC2HEX(A3)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="N3" s="7"/>
+      <c r="N3" s="8"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7" t="s">
+      <c r="T3" s="8"/>
+      <c r="U3" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="V3" s="7"/>
+      <c r="V3" s="8"/>
       <c r="W3" s="4"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="1"/>
@@ -2260,18 +3136,18 @@
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7" t="str">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -2293,18 +3169,18 @@
       <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7" t="str">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -2326,18 +3202,18 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7" t="str">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -2359,18 +3235,18 @@
       <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="str">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -2392,34 +3268,34 @@
       <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="str">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="L8" s="7"/>
+      <c r="L8" s="8"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="7" t="s">
+      <c r="S8" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="T8" s="7"/>
+      <c r="T8" s="8"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -2431,18 +3307,18 @@
       <c r="A9" s="9">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="str">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -2464,18 +3340,18 @@
       <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="str">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -2497,18 +3373,18 @@
       <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="str">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -2530,40 +3406,40 @@
       <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="str">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="L12" s="7"/>
+      <c r="L12" s="8"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="11" t="s">
+      <c r="Q12" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="R12" s="11"/>
+      <c r="R12" s="6"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
-      <c r="W12" s="7" t="s">
+      <c r="W12" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="X12" s="8"/>
+      <c r="X12" s="10"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
@@ -2571,38 +3447,38 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="str">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="11" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="L13" s="11" t="s">
+      <c r="L13" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7" t="s">
+      <c r="N13" s="8"/>
+      <c r="O13" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="11" t="s">
+      <c r="P13" s="8"/>
+      <c r="Q13" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="R13" s="11"/>
+      <c r="R13" s="6"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
@@ -2616,32 +3492,32 @@
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="str">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
       <c r="K14" s="6" t="s">
         <v>115</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -2655,38 +3531,38 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="str">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
       <c r="K15" s="6" t="s">
         <v>115</v>
       </c>
       <c r="L15" s="6"/>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7" t="s">
+      <c r="N15" s="8"/>
+      <c r="O15" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="P15" s="7"/>
+      <c r="P15" s="8"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="7" t="s">
+      <c r="S15" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="T15" s="7"/>
+      <c r="T15" s="8"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
@@ -2698,18 +3574,18 @@
       <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7" t="str">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
@@ -2731,18 +3607,18 @@
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7" t="str">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="str">
         <f t="shared" ref="C17:C28" si="1">DEC2HEX(A17)</f>
         <v>F</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -2764,18 +3640,18 @@
       <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7" t="str">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="str">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -2797,18 +3673,18 @@
       <c r="A19" s="9">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="str">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="str">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -2830,18 +3706,18 @@
       <c r="A20" s="9">
         <v>18</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="str">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8" t="str">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -2863,18 +3739,18 @@
       <c r="A21" s="9">
         <v>19</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="str">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8" t="str">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -2896,18 +3772,18 @@
       <c r="A22" s="9">
         <v>20</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7" t="str">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="str">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -2929,18 +3805,18 @@
       <c r="A23" s="9">
         <v>21</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7" t="str">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="str">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -2962,18 +3838,18 @@
       <c r="A24" s="9">
         <v>22</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7" t="str">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="str">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -2995,18 +3871,18 @@
       <c r="A25" s="9">
         <v>23</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7" t="str">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8" t="str">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -3028,18 +3904,18 @@
       <c r="A26" s="9">
         <v>24</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7" t="str">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8" t="str">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -3061,18 +3937,18 @@
       <c r="A27" s="9">
         <v>25</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7" t="str">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8" t="str">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -3094,18 +3970,18 @@
       <c r="A28" s="9">
         <v>26</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7" t="str">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8" t="str">
         <f t="shared" si="1"/>
         <v>1A</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -3293,84 +4169,14 @@
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:J3"/>
     <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C14:D14"/>
@@ -3386,19 +4192,89 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="K8:L8"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0253E003-5A06-488A-A834-EFA5548C0B3D}">
   <dimension ref="A1:V46"/>
   <sheetViews>
@@ -3440,83 +4316,83 @@
       <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="7">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="1" t="s">
         <v>63</v>
       </c>
@@ -3529,778 +4405,743 @@
       <c r="G4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="7">
         <v>20</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10"/>
+      <c r="E21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="10"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="10"/>
-      <c r="V29" s="10"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
-      <c r="V30" s="10"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
-      <c r="T31" s="10"/>
-      <c r="U31" s="10"/>
-      <c r="V31" s="10"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10"/>
-      <c r="T32" s="10"/>
-      <c r="U32" s="10"/>
-      <c r="V32" s="10"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="10"/>
-      <c r="V34" s="10"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="10"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="10"/>
-      <c r="U37" s="10"/>
-      <c r="V37" s="10"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
-      <c r="T38" s="10"/>
-      <c r="U38" s="10"/>
-      <c r="V38" s="10"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
-      <c r="V39" s="10"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
-      <c r="T40" s="10"/>
-      <c r="U40" s="10"/>
-      <c r="V40" s="10"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
-      <c r="T41" s="10"/>
-      <c r="U41" s="10"/>
-      <c r="V41" s="10"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="10"/>
-      <c r="T42" s="10"/>
-      <c r="U42" s="10"/>
-      <c r="V42" s="10"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="7"/>
+      <c r="V42" s="7"/>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
-      <c r="T43" s="10"/>
-      <c r="U43" s="10"/>
-      <c r="V43" s="10"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7"/>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
-      <c r="T44" s="10"/>
-      <c r="U44" s="10"/>
-      <c r="V44" s="10"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="7"/>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7"/>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-      <c r="S45" s="10"/>
-      <c r="T45" s="10"/>
-      <c r="U45" s="10"/>
-      <c r="V45" s="10"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-      <c r="S46" s="10"/>
-      <c r="T46" s="10"/>
-      <c r="U46" s="10"/>
-      <c r="V46" s="10"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="J15:V15"/>
-    <mergeCell ref="J16:V16"/>
-    <mergeCell ref="J17:V17"/>
-    <mergeCell ref="J18:V18"/>
-    <mergeCell ref="J19:V19"/>
-    <mergeCell ref="J20:V20"/>
-    <mergeCell ref="J21:V21"/>
-    <mergeCell ref="J22:V22"/>
-    <mergeCell ref="J23:V23"/>
-    <mergeCell ref="J24:V24"/>
-    <mergeCell ref="J25:V25"/>
-    <mergeCell ref="J26:V26"/>
-    <mergeCell ref="J27:V27"/>
-    <mergeCell ref="J28:V28"/>
-    <mergeCell ref="J29:V29"/>
+    <mergeCell ref="J45:V45"/>
+    <mergeCell ref="J46:V46"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="J40:V40"/>
+    <mergeCell ref="J41:V41"/>
+    <mergeCell ref="J42:V42"/>
+    <mergeCell ref="J43:V43"/>
+    <mergeCell ref="J44:V44"/>
+    <mergeCell ref="J35:V35"/>
+    <mergeCell ref="J36:V36"/>
+    <mergeCell ref="J37:V37"/>
+    <mergeCell ref="J38:V38"/>
+    <mergeCell ref="J39:V39"/>
+    <mergeCell ref="J30:V30"/>
+    <mergeCell ref="J31:V31"/>
+    <mergeCell ref="J32:V32"/>
     <mergeCell ref="J33:V33"/>
     <mergeCell ref="J34:V34"/>
     <mergeCell ref="J1:V1"/>
@@ -4317,28 +5158,63 @@
     <mergeCell ref="J12:V12"/>
     <mergeCell ref="J13:V13"/>
     <mergeCell ref="J14:V14"/>
-    <mergeCell ref="J45:V45"/>
-    <mergeCell ref="J46:V46"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="J40:V40"/>
-    <mergeCell ref="J41:V41"/>
-    <mergeCell ref="J42:V42"/>
-    <mergeCell ref="J43:V43"/>
-    <mergeCell ref="J44:V44"/>
-    <mergeCell ref="J35:V35"/>
-    <mergeCell ref="J36:V36"/>
-    <mergeCell ref="J37:V37"/>
-    <mergeCell ref="J38:V38"/>
-    <mergeCell ref="J39:V39"/>
-    <mergeCell ref="J30:V30"/>
-    <mergeCell ref="J31:V31"/>
-    <mergeCell ref="J32:V32"/>
+    <mergeCell ref="J25:V25"/>
+    <mergeCell ref="J26:V26"/>
+    <mergeCell ref="J27:V27"/>
+    <mergeCell ref="J28:V28"/>
+    <mergeCell ref="J29:V29"/>
+    <mergeCell ref="J20:V20"/>
+    <mergeCell ref="J21:V21"/>
+    <mergeCell ref="J22:V22"/>
+    <mergeCell ref="J23:V23"/>
+    <mergeCell ref="J24:V24"/>
+    <mergeCell ref="J15:V15"/>
+    <mergeCell ref="J16:V16"/>
+    <mergeCell ref="J17:V17"/>
+    <mergeCell ref="J18:V18"/>
+    <mergeCell ref="J19:V19"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F820F2B8-A0D6-407B-8331-DFA89AFEF3E6}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
@@ -4381,251 +5257,250 @@
       <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="7">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="7"/>
       <c r="G2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="7"/>
       <c r="G3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="1" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="J5:Z5"/>
-    <mergeCell ref="J3:Z3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="J4:Z4"/>
-    <mergeCell ref="J1:Z1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="J2:Z2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="J6:Z6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -4635,13 +5510,14 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="J6:Z6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J5:Z5"/>
+    <mergeCell ref="J3:Z3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="J4:Z4"/>
+    <mergeCell ref="J1:Z1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="J2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reworking the assembler and other things
</commit_message>
<xml_diff>
--- a/BES-8-CPU/CPU-SPECS/Stack.xlsx
+++ b/BES-8-CPU/CPU-SPECS/Stack.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjorn\Desktop\BES-8-CPU\CPUs\BES-8-CPU\CPU-SPECS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCF905E-6B64-4964-A354-44D5D0C92B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACFBBDF-9D87-46D5-9949-DB76ABFB84E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{60BD8EC7-1CE0-4AB1-8C1D-843B2C9E47D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{60BD8EC7-1CE0-4AB1-8C1D-843B2C9E47D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="180">
   <si>
     <t>A</t>
   </si>
@@ -481,10 +481,106 @@
     <t>R4</t>
   </si>
   <si>
-    <t>10FFE</t>
-  </si>
-  <si>
-    <t>10FFF</t>
+    <t>Conv dec to hex</t>
+  </si>
+  <si>
+    <t>ushort dec</t>
+  </si>
+  <si>
+    <t>return sbyte Exit_Code</t>
+  </si>
+  <si>
+    <t>char c</t>
+  </si>
+  <si>
+    <t>put a char on the video output</t>
+  </si>
+  <si>
+    <t>byte count</t>
+  </si>
+  <si>
+    <t>return char* hex</t>
+  </si>
+  <si>
+    <t>E900</t>
+  </si>
+  <si>
+    <t>E901</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>PMB</t>
+  </si>
+  <si>
+    <t>0x114</t>
+  </si>
+  <si>
+    <t>0000001111111111</t>
+  </si>
+  <si>
+    <t>70a</t>
+  </si>
+  <si>
+    <t>70b</t>
+  </si>
+  <si>
+    <t>In disk</t>
+  </si>
+  <si>
+    <t>70c</t>
+  </si>
+  <si>
+    <t>70d</t>
+  </si>
+  <si>
+    <t>70e</t>
+  </si>
+  <si>
+    <t>Char</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>Sectors</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>disk</t>
+  </si>
+  <si>
+    <t>ushort page</t>
+  </si>
+  <si>
+    <t>Read Byte</t>
+  </si>
+  <si>
+    <t>uint address</t>
+  </si>
+  <si>
+    <t>uint* address</t>
+  </si>
+  <si>
+    <t>Write Byte</t>
+  </si>
+  <si>
+    <t>Byte Data</t>
+  </si>
+  <si>
+    <t>uint count</t>
+  </si>
+  <si>
+    <t>ushort StartAddress</t>
+  </si>
+  <si>
+    <t>ushort address</t>
+  </si>
+  <si>
+    <t>Read Count</t>
   </si>
 </sst>
 </file>
@@ -508,7 +604,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -621,11 +717,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -652,28 +768,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1864,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFC2456-8F03-4C66-81C2-5B49407479C5}">
-  <dimension ref="A1:X43"/>
+  <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,19 +1996,20 @@
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -1920,10 +2042,8 @@
         <v>33</v>
       </c>
       <c r="S1" s="1"/>
-      <c r="T1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" s="12"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E2" s="3"/>
@@ -1941,18 +2061,14 @@
         <f>DEC2HEX(N2)</f>
         <v>1</v>
       </c>
-      <c r="P2" t="s">
-        <v>33</v>
+      <c r="Q2" t="s">
+        <v>7</v>
       </c>
       <c r="S2" s="3"/>
-      <c r="T2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="12"/>
-      <c r="W2" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="X2" s="12"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I3" s="2"/>
@@ -1964,23 +2080,6 @@
         <f t="shared" ref="O3:O30" si="0">DEC2HEX(N3)</f>
         <v>2</v>
       </c>
-      <c r="P3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" t="str">
-        <f>DEC2HEX(U3)</f>
-        <v>32000</v>
-      </c>
-      <c r="U3">
-        <v>204800</v>
-      </c>
-      <c r="W3">
-        <v>32000</v>
-      </c>
-      <c r="X3">
-        <f>HEX2DEC(W3)</f>
-        <v>204800</v>
-      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="N4" s="1">
@@ -1990,19 +2089,6 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="T4" t="str">
-        <f t="shared" ref="T4:T18" si="1">DEC2HEX(U4)</f>
-        <v>32001</v>
-      </c>
-      <c r="U4">
-        <v>204801</v>
-      </c>
-      <c r="W4">
-        <v>32001</v>
-      </c>
-      <c r="X4">
-        <v>225281</v>
-      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="N5" s="1">
@@ -2012,19 +2098,6 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="T5" t="str">
-        <f t="shared" si="1"/>
-        <v>32002</v>
-      </c>
-      <c r="U5">
-        <v>204802</v>
-      </c>
-      <c r="W5">
-        <v>32002</v>
-      </c>
-      <c r="X5">
-        <v>225282</v>
-      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2036,11 +2109,11 @@
       <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="I6" t="s">
-        <v>146</v>
-      </c>
-      <c r="J6">
-        <v>20</v>
+      <c r="I6">
+        <v>2000</v>
+      </c>
+      <c r="J6" t="s">
+        <v>157</v>
       </c>
       <c r="N6" s="1">
         <v>5</v>
@@ -2048,19 +2121,6 @@
       <c r="O6" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
-      </c>
-      <c r="T6" t="str">
-        <f t="shared" si="1"/>
-        <v>32003</v>
-      </c>
-      <c r="U6">
-        <v>204803</v>
-      </c>
-      <c r="W6">
-        <v>32003</v>
-      </c>
-      <c r="X6">
-        <v>225283</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -2069,13 +2129,13 @@
       </c>
       <c r="C7" t="str">
         <f>IF(B7&lt;&gt;0,LOOKUP(HEX2DEC(B7),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C8),2),DEC2HEX(HEX2DEC(C9),2)))</f>
-        <v>0020</v>
+        <v>0000</v>
       </c>
       <c r="I7" t="s">
-        <v>147</v>
-      </c>
-      <c r="J7">
-        <v>10</v>
+        <v>153</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="N7" s="1">
         <v>6</v>
@@ -2083,19 +2143,6 @@
       <c r="O7" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
-      </c>
-      <c r="T7" t="str">
-        <f t="shared" si="1"/>
-        <v>32004</v>
-      </c>
-      <c r="U7">
-        <v>204804</v>
-      </c>
-      <c r="W7">
-        <v>32004</v>
-      </c>
-      <c r="X7">
-        <v>225284</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -2105,25 +2152,15 @@
       <c r="C8">
         <v>0</v>
       </c>
+      <c r="I8" t="s">
+        <v>154</v>
+      </c>
       <c r="N8" s="1">
         <v>7</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
-      </c>
-      <c r="T8" t="str">
-        <f t="shared" si="1"/>
-        <v>32005</v>
-      </c>
-      <c r="U8">
-        <v>204805</v>
-      </c>
-      <c r="W8">
-        <v>32005</v>
-      </c>
-      <c r="X8">
-        <v>225285</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -2131,7 +2168,7 @@
         <v>40</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="N9" s="1">
         <v>8</v>
@@ -2139,19 +2176,6 @@
       <c r="O9" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
-      </c>
-      <c r="T9" t="str">
-        <f t="shared" si="1"/>
-        <v>32006</v>
-      </c>
-      <c r="U9">
-        <v>204806</v>
-      </c>
-      <c r="W9">
-        <v>32006</v>
-      </c>
-      <c r="X9">
-        <v>225286</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -2169,13 +2193,6 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="T10" t="str">
-        <f t="shared" si="1"/>
-        <v>32007</v>
-      </c>
-      <c r="U10">
-        <v>204807</v>
-      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2190,13 +2207,6 @@
       <c r="O11" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
-      </c>
-      <c r="T11" t="str">
-        <f t="shared" si="1"/>
-        <v>32008</v>
-      </c>
-      <c r="U11">
-        <v>204808</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -2215,13 +2225,6 @@
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
-      <c r="T12" t="str">
-        <f t="shared" si="1"/>
-        <v>32009</v>
-      </c>
-      <c r="U12">
-        <v>204809</v>
-      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2240,13 +2243,6 @@
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
-      <c r="T13" t="str">
-        <f t="shared" si="1"/>
-        <v>3200A</v>
-      </c>
-      <c r="U13">
-        <v>204810</v>
-      </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2264,13 +2260,6 @@
         <f t="shared" si="0"/>
         <v>D</v>
       </c>
-      <c r="T14" t="str">
-        <f t="shared" si="1"/>
-        <v>3200B</v>
-      </c>
-      <c r="U14">
-        <v>204811</v>
-      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2279,21 +2268,21 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
       <c r="N15" s="1">
         <v>14</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
-      </c>
-      <c r="T15" t="str">
-        <f t="shared" si="1"/>
-        <v>3200C</v>
-      </c>
-      <c r="U15">
-        <v>204812</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -2304,8 +2293,18 @@
         <f>IF(B16&lt;&gt;0,LOOKUP(HEX2DEC(B16),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C17),2),DEC2HEX(HEX2DEC(C18),2)))</f>
         <v>0000</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
       <c r="N16" s="1">
         <v>15</v>
       </c>
@@ -2313,23 +2312,26 @@
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="T16" t="str">
-        <f t="shared" si="1"/>
-        <v>3200D</v>
-      </c>
-      <c r="U16">
-        <v>204813</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
       <c r="N17" s="1">
         <v>16</v>
       </c>
@@ -2337,29 +2339,14 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="T17" t="str">
-        <f t="shared" si="1"/>
-        <v>3200E</v>
-      </c>
-      <c r="U17">
-        <v>204814</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="I18">
-        <v>11000</v>
-      </c>
-      <c r="J18">
-        <v>30</v>
-      </c>
       <c r="N18" s="1">
         <v>17</v>
       </c>
@@ -2367,15 +2354,8 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="T18" t="str">
-        <f t="shared" si="1"/>
-        <v>3200F</v>
-      </c>
-      <c r="U18">
-        <v>204815</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2384,14 +2364,6 @@
         <v>0000</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="I19">
-        <v>11001</v>
-      </c>
-      <c r="J19">
-        <v>20</v>
-      </c>
       <c r="N19" s="1">
         <v>18</v>
       </c>
@@ -2400,21 +2372,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="I20">
-        <v>11002</v>
-      </c>
-      <c r="J20">
-        <v>10</v>
-      </c>
       <c r="N20" s="1">
         <v>19</v>
       </c>
@@ -2423,15 +2387,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
       <c r="N21" s="1">
         <v>20</v>
       </c>
@@ -2440,16 +2402,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="C22" t="str">
         <f>IF(B22&lt;&gt;0,LOOKUP(HEX2DEC(B22),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C23),2),DEC2HEX(HEX2DEC(C24),2)))</f>
-        <v>0000</v>
-      </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+        <v>0101</v>
+      </c>
+      <c r="F22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22">
+        <v>16</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
       <c r="N22" s="1">
         <v>21</v>
       </c>
@@ -2458,15 +2430,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
       <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23">
+        <v>17</v>
+      </c>
+      <c r="H23">
         <v>0</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="I23">
+        <v>0</v>
+      </c>
       <c r="N23" s="1">
         <v>22</v>
       </c>
@@ -2475,26 +2460,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
       <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24">
+        <v>18</v>
+      </c>
+      <c r="H24">
         <v>0</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" t="s">
-        <v>63</v>
-      </c>
       <c r="I24">
-        <v>41010</v>
-      </c>
-      <c r="J24">
-        <f>HEX2DEC(I24)</f>
-        <v>266256</v>
-      </c>
-      <c r="K24">
         <v>0</v>
       </c>
       <c r="N24" s="1">
@@ -2505,7 +2487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2515,19 +2497,6 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25">
-        <v>41011</v>
-      </c>
-      <c r="J25">
-        <f t="shared" ref="J25:J26" si="2">HEX2DEC(I25)</f>
-        <v>266257</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
       <c r="N25" s="1">
         <v>24</v>
       </c>
@@ -2536,7 +2505,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -2545,16 +2514,6 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" t="s">
-        <v>65</v>
-      </c>
-      <c r="I26">
-        <v>41012</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="2"/>
-        <v>266258</v>
-      </c>
       <c r="N26" s="1">
         <v>25</v>
       </c>
@@ -2563,7 +2522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -2580,13 +2539,13 @@
         <v>1A</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
       <c r="C28" t="str">
         <f>IF(B28&lt;&gt;0,LOOKUP(HEX2DEC(B28),$N$2:$N$30,$P$6:$P$30),_xlfn.CONCAT(DEC2HEX(HEX2DEC(C29),2),DEC2HEX(HEX2DEC(C30),2)))</f>
-        <v>0020</v>
+        <v>0000</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -2599,7 +2558,7 @@
         <v>1B</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -2617,12 +2576,12 @@
         <v>1C</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>51</v>
       </c>
       <c r="C30">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2635,30 +2594,50 @@
         <v>1D</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31">
+        <v>800</v>
+      </c>
+      <c r="D31" t="s">
+        <v>168</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F32" s="1"/>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>161</v>
+      </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" t="s">
-        <v>57</v>
+      <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2666,16 +2645,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
+        <v>155</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2683,58 +2656,87 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36">
+        <v>156</v>
+      </c>
+      <c r="F36" s="1">
+        <v>702</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C36">
+      <c r="H36" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F37" s="1">
+        <v>703</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F38" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F40" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40">
         <v>0</v>
       </c>
-      <c r="D36">
+      <c r="H40" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F41" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G41">
         <v>0</v>
       </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41">
-        <v>16</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
+      <c r="H41" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F42" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42">
-        <v>17</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>18</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
+      <c r="H42" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3138,8 +3140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB048CF3-8843-4B40-B9E5-99F22F345F1B}">
   <dimension ref="A1:AB39"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3149,29 +3151,32 @@
     <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.140625" customWidth="1"/>
     <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="10" t="s">
         <v>40</v>
       </c>
@@ -3231,24 +3236,24 @@
       <c r="A2" s="16">
         <v>224</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14" t="str">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15" t="str">
         <f>DEC2HEX(A2)</f>
         <v>E0</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="14"/>
+      <c r="L2" s="15"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
@@ -3270,40 +3275,40 @@
       <c r="A3" s="16">
         <v>225</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14" t="str">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="str">
         <f t="shared" ref="C3:C16" si="0">DEC2HEX(A3)</f>
         <v>E1</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="14"/>
+      <c r="N3" s="15"/>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
-      <c r="S3" s="14" t="s">
+      <c r="S3" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14" t="s">
+      <c r="T3" s="15"/>
+      <c r="U3" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="V3" s="14"/>
+      <c r="V3" s="15"/>
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
@@ -3315,18 +3320,18 @@
       <c r="A4" s="16">
         <v>226</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14" t="str">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E2</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
@@ -3350,18 +3355,18 @@
       <c r="A5" s="16">
         <v>227</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14" t="str">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E3</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -3385,18 +3390,18 @@
       <c r="A6" s="16">
         <v>228</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14" t="str">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E4</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -3420,18 +3425,18 @@
       <c r="A7" s="16">
         <v>229</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14" t="str">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E5</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -3455,35 +3460,37 @@
       <c r="A8" s="16">
         <v>230</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14" t="str">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E6</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="15"/>
+      <c r="E8" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14" t="s">
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="L8" s="14"/>
+      <c r="L8" s="15"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
-      <c r="S8" s="14" t="s">
+      <c r="S8" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="T8" s="14"/>
-      <c r="U8" s="7"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="7" t="s">
+        <v>151</v>
+      </c>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
@@ -3496,32 +3503,38 @@
       <c r="A9" s="16">
         <v>231</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14" t="str">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E7</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="L9" s="15"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
+      <c r="W9" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="X9" s="15"/>
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="8"/>
@@ -3531,18 +3544,18 @@
       <c r="A10" s="16">
         <v>232</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14" t="str">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E8</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -3566,30 +3579,42 @@
       <c r="A11" s="16">
         <v>233</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14" t="str">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15" t="str">
         <f t="shared" si="0"/>
         <v>E9</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="L11" s="15"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
+      <c r="N11" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
       <c r="Y11" s="7"/>
@@ -3601,30 +3626,30 @@
       <c r="A12" s="16">
         <v>234</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14" t="str">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>EA</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="L12" s="14"/>
+      <c r="L12" s="15"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="14" t="s">
+      <c r="O12" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="P12" s="14"/>
+      <c r="P12" s="15"/>
       <c r="Q12" s="8" t="s">
         <v>86</v>
       </c>
@@ -3635,10 +3660,10 @@
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
-      <c r="W12" s="14" t="s">
+      <c r="W12" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="X12" s="14"/>
+      <c r="X12" s="15"/>
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="8"/>
@@ -3648,32 +3673,32 @@
       <c r="A13" s="16">
         <v>235</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14" t="str">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15" t="str">
         <f t="shared" si="0"/>
         <v>EB</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14" t="s">
+      <c r="L13" s="15"/>
+      <c r="M13" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14" t="s">
+      <c r="N13" s="15"/>
+      <c r="O13" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="P13" s="14"/>
+      <c r="P13" s="15"/>
       <c r="Q13" s="8" t="s">
         <v>86</v>
       </c>
@@ -3695,20 +3720,20 @@
       <c r="A14" s="16">
         <v>236</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14" t="str">
-        <f t="shared" si="0"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15" t="str">
+        <f>DEC2HEX(A14)</f>
         <v>EC</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="8" t="s">
         <v>86</v>
       </c>
@@ -3717,10 +3742,10 @@
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
-      <c r="O14" s="14" t="s">
+      <c r="O14" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="P14" s="14"/>
+      <c r="P14" s="15"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="7"/>
@@ -3738,38 +3763,38 @@
       <c r="A15" s="16">
         <v>237</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14" t="str">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15" t="str">
         <f t="shared" si="0"/>
         <v>ED</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="8" t="s">
         <v>86</v>
       </c>
       <c r="L15" s="8"/>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14" t="s">
+      <c r="N15" s="15"/>
+      <c r="O15" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="P15" s="14"/>
+      <c r="P15" s="15"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="14" t="s">
+      <c r="S15" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="T15" s="14"/>
+      <c r="T15" s="15"/>
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
       <c r="W15" s="7"/>
@@ -3783,18 +3808,18 @@
       <c r="A16" s="16">
         <v>238</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14" t="str">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15" t="str">
         <f t="shared" si="0"/>
         <v>EE</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -3818,18 +3843,18 @@
       <c r="A17" s="16">
         <v>239</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14" t="str">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15" t="str">
         <f t="shared" ref="C17:C28" si="1">DEC2HEX(A17)</f>
         <v>EF</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -3853,18 +3878,18 @@
       <c r="A18" s="16">
         <v>240</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14" t="str">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F0</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -3888,18 +3913,18 @@
       <c r="A19" s="16">
         <v>241</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14" t="str">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F1</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -3923,18 +3948,18 @@
       <c r="A20" s="16">
         <v>242</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14" t="str">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F2</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
@@ -3958,18 +3983,18 @@
       <c r="A21" s="16">
         <v>243</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14" t="str">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F3</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
@@ -3993,18 +4018,18 @@
       <c r="A22" s="16">
         <v>244</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14" t="str">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F4</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
@@ -4028,18 +4053,18 @@
       <c r="A23" s="16">
         <v>245</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14" t="str">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F5</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
@@ -4063,18 +4088,18 @@
       <c r="A24" s="16">
         <v>246</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14" t="str">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F6</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
@@ -4098,18 +4123,18 @@
       <c r="A25" s="16">
         <v>247</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14" t="str">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F7</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -4133,18 +4158,18 @@
       <c r="A26" s="16">
         <v>248</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14" t="str">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F8</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
@@ -4168,18 +4193,18 @@
       <c r="A27" s="16">
         <v>249</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14" t="str">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15" t="str">
         <f t="shared" si="1"/>
         <v>F9</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
@@ -4203,30 +4228,34 @@
       <c r="A28" s="16">
         <v>250</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14" t="str">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15" t="str">
         <f t="shared" si="1"/>
         <v>FA</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14" t="s">
+      <c r="D28" s="15"/>
+      <c r="E28" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
+      <c r="S28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="T28" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="U28" s="7"/>
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
@@ -4242,22 +4271,24 @@
       <c r="A29" s="16">
         <v>251</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14" t="str">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15" t="str">
         <f t="shared" ref="C29:C33" si="2">DEC2HEX(A29)</f>
         <v>FB</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14" t="s">
+      <c r="D29" s="15"/>
+      <c r="E29" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="L29" s="19"/>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
       <c r="O29" s="7"/>
@@ -4279,18 +4310,18 @@
       <c r="A30" s="16">
         <v>252</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14" t="str">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15" t="str">
         <f t="shared" si="2"/>
         <v>FC</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
@@ -4314,18 +4345,18 @@
       <c r="A31" s="16">
         <v>253</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14" t="str">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15" t="str">
         <f t="shared" si="2"/>
         <v>FD</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
@@ -4349,18 +4380,18 @@
       <c r="A32" s="16">
         <v>254</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14" t="str">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15" t="str">
         <f t="shared" si="2"/>
         <v>FE</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
@@ -4384,18 +4415,18 @@
       <c r="A33" s="16">
         <v>255</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14" t="str">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15" t="str">
         <f t="shared" si="2"/>
         <v>FF</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
@@ -4490,77 +4521,29 @@
       <c r="X39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="116">
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E23:J23"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="E20:J20"/>
-    <mergeCell ref="E21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
+  <mergeCells count="124">
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="W12:X12"/>
@@ -4583,41 +4566,98 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="S9:T9"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E5:J5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="E8:J8"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="E26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE1AE75-ADB5-4F57-891A-349E9B560230}">
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4627,27 +4667,28 @@
     <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9.140625" customWidth="1"/>
     <col min="29" max="29" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="K1" s="4" t="s">
         <v>40</v>
       </c>
@@ -4690,31 +4731,35 @@
       <c r="X1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18" t="str">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="str">
         <f>DEC2HEX(A2)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="18"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -4727,70 +4772,80 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="5"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18" t="str">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="str">
         <f t="shared" ref="C3:C29" si="0">DEC2HEX(A3)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
       <c r="K3" s="6" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="L3" s="6"/>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="18"/>
+      <c r="N3" s="6"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="18" t="s">
+      <c r="S3" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18" t="s">
+      <c r="T3" s="20"/>
+      <c r="U3" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="V3" s="18"/>
+      <c r="V3" s="20"/>
       <c r="W3" s="4"/>
       <c r="X3" s="5"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="Y3" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="str">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -4803,58 +4858,66 @@
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="5"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
         <v>3</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18" t="str">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
       <c r="W5" s="4"/>
       <c r="X5" s="5"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
         <v>4</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18" t="str">
+      <c r="B6" s="20"/>
+      <c r="C6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -4869,25 +4932,29 @@
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
       <c r="X6" s="5"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
         <v>5</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="str">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -4902,58 +4969,66 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
       <c r="X7" s="5"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
         <v>6</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18" t="str">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="5"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
         <v>7</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18" t="str">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -4968,25 +5043,29 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="5"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
         <v>8</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18" t="str">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -5001,25 +5080,29 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="5"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
+      <c r="AB10" s="14"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="14"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
         <v>9</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18" t="str">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -5034,27 +5117,31 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="5"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="14"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
         <v>10</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18" t="str">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -5065,33 +5152,37 @@
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+      <c r="W12" s="6"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="14"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
         <v>11</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18" t="str">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="4"/>
@@ -5100,94 +5191,112 @@
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="5"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
         <v>12</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18" t="str">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="5"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
         <v>13</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="str">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="5"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
         <v>14</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="str">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="L16" s="20"/>
+      <c r="M16" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="N16" s="6"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -5199,31 +5308,43 @@
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="5"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="14"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
         <v>15</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18" t="str">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="O17" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="P17" s="20"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
@@ -5232,91 +5353,129 @@
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="5"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="14"/>
+      <c r="AA17" s="14"/>
+      <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="14"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
         <v>16</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="str">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="5"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
         <v>17</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18" t="str">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M19" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="T19" s="20"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="5"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+      <c r="Y19" s="22"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="14"/>
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="14"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
         <v>18</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18" t="str">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -5331,25 +5490,29 @@
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="5"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="Y20" s="22"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
         <v>19</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18" t="str">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -5364,25 +5527,29 @@
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="5"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="14"/>
+      <c r="AA21" s="14"/>
+      <c r="AB21" s="14"/>
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="14"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
         <v>20</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18" t="str">
+      <c r="B22" s="20"/>
+      <c r="C22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -5397,25 +5564,29 @@
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
       <c r="X22" s="5"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+      <c r="Y22" s="22"/>
+      <c r="Z22" s="14"/>
+      <c r="AA22" s="14"/>
+      <c r="AB22" s="14"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="14"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
         <v>21</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18" t="str">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -5430,25 +5601,29 @@
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
       <c r="X23" s="5"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="14"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
         <v>22</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18" t="str">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20" t="str">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -5463,25 +5638,29 @@
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="5"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
+      <c r="Y24" s="22"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="14"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
         <v>23</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18" t="str">
+      <c r="B25" s="20"/>
+      <c r="C25" s="20" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -5496,25 +5675,29 @@
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="5"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+      <c r="Y25" s="22"/>
+      <c r="Z25" s="14"/>
+      <c r="AA25" s="14"/>
+      <c r="AB25" s="14"/>
+      <c r="AC25" s="14"/>
+      <c r="AD25" s="14"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
         <v>24</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18" t="str">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -5529,25 +5712,29 @@
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
       <c r="X26" s="5"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+      <c r="Y26" s="22"/>
+      <c r="Z26" s="14"/>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="14"/>
+      <c r="AC26" s="14"/>
+      <c r="AD26" s="14"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
         <v>25</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18" t="str">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -5562,27 +5749,31 @@
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="5"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
+      <c r="Y27" s="22"/>
+      <c r="Z27" s="14"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="14"/>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="14"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
         <v>26</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18" t="str">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20" t="str">
         <f t="shared" si="0"/>
         <v>1A</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="O28" s="4"/>
@@ -5595,25 +5786,29 @@
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="5"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
+      <c r="Y28" s="22"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="14"/>
+      <c r="AC28" s="14"/>
+      <c r="AD28" s="14"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="21">
         <v>27</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18" t="str">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20" t="str">
         <f t="shared" si="0"/>
         <v>1B</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -5628,10 +5823,14 @@
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
       <c r="X29" s="5"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="14"/>
+      <c r="AB29" s="14"/>
+      <c r="AC29" s="14"/>
+      <c r="AD29" s="14"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -5656,10 +5855,8 @@
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -5684,10 +5881,8 @@
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -5712,8 +5907,6 @@
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -5740,8 +5933,6 @@
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
@@ -5772,20 +5963,90 @@
       <c r="Z34" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="108">
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:J25"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:J23"/>
+  <mergeCells count="127">
+    <mergeCell ref="Y29:AD29"/>
+    <mergeCell ref="Y1:AD1"/>
+    <mergeCell ref="Y20:AD20"/>
+    <mergeCell ref="Y21:AD21"/>
+    <mergeCell ref="Y22:AD22"/>
+    <mergeCell ref="Y23:AD23"/>
+    <mergeCell ref="Y24:AD24"/>
+    <mergeCell ref="Y25:AD25"/>
+    <mergeCell ref="Y26:AD26"/>
+    <mergeCell ref="Y27:AD27"/>
+    <mergeCell ref="Y28:AD28"/>
+    <mergeCell ref="Y11:AD11"/>
+    <mergeCell ref="Y12:AD12"/>
+    <mergeCell ref="Y13:AD13"/>
+    <mergeCell ref="Y14:AD14"/>
+    <mergeCell ref="Y15:AD15"/>
+    <mergeCell ref="Y16:AD16"/>
+    <mergeCell ref="Y17:AD17"/>
+    <mergeCell ref="Y18:AD18"/>
+    <mergeCell ref="Y19:AD19"/>
+    <mergeCell ref="Y3:AD3"/>
+    <mergeCell ref="Y2:AD2"/>
+    <mergeCell ref="Y4:AD4"/>
+    <mergeCell ref="Y5:AD5"/>
+    <mergeCell ref="Y6:AD6"/>
+    <mergeCell ref="Y7:AD7"/>
+    <mergeCell ref="Y8:AD8"/>
+    <mergeCell ref="Y9:AD9"/>
+    <mergeCell ref="Y10:AD10"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:J15"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:J29"/>
@@ -5798,6 +6059,26 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:J28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:J25"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:J24"/>
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C21:D21"/>
@@ -5810,77 +6091,6 @@
     <mergeCell ref="E19:J19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:J14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:J15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5903,32 +6113,32 @@
       <c r="A1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
       <c r="H2" t="s">
         <v>124</v>
       </c>
@@ -5943,14 +6153,14 @@
       <c r="A3" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
       <c r="H3" t="s">
         <v>130</v>
       </c>
@@ -5965,14 +6175,14 @@
       <c r="A4" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="H4" t="s">
         <v>129</v>
       </c>
@@ -5984,27 +6194,27 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
       <c r="H6" t="s">
         <v>124</v>
       </c>
@@ -6016,27 +6226,27 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
       <c r="H8" t="s">
         <v>124</v>
       </c>
@@ -6048,27 +6258,27 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
       <c r="H10" t="s">
         <v>124</v>
       </c>
@@ -6083,14 +6293,14 @@
       <c r="A11" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="H11" t="s">
         <v>126</v>
       </c>
@@ -6105,14 +6315,14 @@
       <c r="A12" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
       <c r="H12" t="s">
         <v>130</v>
       </c>
@@ -6127,14 +6337,14 @@
       <c r="A13" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
       <c r="H13" t="s">
         <v>132</v>
       </c>
@@ -6149,14 +6359,14 @@
       <c r="A14" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
       <c r="H14" t="s">
         <v>133</v>
       </c>
@@ -6171,14 +6381,14 @@
       <c r="A15" t="s">
         <v>117</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
       <c r="H15" t="s">
         <v>135</v>
       </c>
@@ -6191,22 +6401,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B14:G14"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>